<commit_message>
Excel - 3. feladat
</commit_message>
<xml_diff>
--- a/ZelenakSz_13.A_lampak.xlsx
+++ b/ZelenakSz_13.A_lampak.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelenaksz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelenaksz\Desktop\cucc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D178CC-643F-43DE-8963-4E40686F0898}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC49CC6-DCAE-4D97-B19A-08ECC659FF75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{83E2134B-7878-4807-8A5C-88B4790D783A}"/>
   </bookViews>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A68BDDD-20BA-41B3-BFB5-B7E05B9F6C62}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -468,599 +468,999 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="str">
+        <f ca="1">MID("ABCDEF", RANDBETWEEN(1,6),1)</f>
+        <v>F</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="str">
         <f>ROW(A2) &amp; "."</f>
         <v>2.</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" ca="1" si="0">MID("ABCDEF", RANDBETWEEN(1,6),1)</f>
+        <v>C</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="str">
-        <f t="shared" ref="A4:A67" si="0">ROW(A3) &amp; "."</f>
+        <f t="shared" ref="A4:A67" si="1">ROW(A3) &amp; "."</f>
         <v>3.</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10.</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12.</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14.</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30.</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31.</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32.</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33.</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34.</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35.</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40.</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41.</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42.</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43.</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44.</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45.</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47.</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48.</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>49.</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50.</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53.</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55.</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57.</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58.</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59.</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>60.</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>62.</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64.</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65.</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66.</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B101" ca="1" si="2">MID("ABCDEF", RANDBETWEEN(1,6),1)</f>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="str">
-        <f t="shared" ref="A68:A101" si="1">ROW(A67) &amp; "."</f>
+        <f t="shared" ref="A68:A101" si="3">ROW(A67) &amp; "."</f>
         <v>67.</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>68.</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>69.</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>70.</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>71.</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>72.</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>73.</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>74.</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>75.</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>76.</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>77.</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>78.</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>79.</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>80.</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>81.</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>82.</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>83.</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>84.</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>85.</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>86.</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>87.</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>88.</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>89.</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>D</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>90.</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>91.</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>92.</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>93.</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>94.</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>95.</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>E</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>96.</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>97.</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>98.</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>99.</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>C</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>100.</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>B</v>
       </c>
     </row>
   </sheetData>

</xml_diff>